<commit_message>
Attendance Info (Ramzor Graphs)
</commit_message>
<xml_diff>
--- a/src/main/resources/Data.xlsx
+++ b/src/main/resources/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yenov segal\Desktop\KodkodAutomation\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yahav\IdeaProjects\Automation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD132CC-5B9B-41EA-B071-CB72C847B290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DAB304-BADB-4651-8E08-0AD8410BBB2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Interview" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <t>noteText:</t>
   </si>
   <si>
-    <t>jhjhjhjhjhjhjhjhjhjhjhjhjhjhjhjhj</t>
+    <t>asasasasasasasasasasasasasasasas</t>
   </si>
 </sst>
 </file>
@@ -54,7 +54,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -63,7 +63,7 @@
       <u/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -72,7 +72,7 @@
       <u/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -384,16 +384,16 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A6" sqref="A6:A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="22.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -401,7 +401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -423,20 +423,20 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>

</xml_diff>